<commit_message>
revert all changes in experiment test data
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_confMatrix.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_confMatrix.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,6 +12,10 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -50,89 +54,22 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -433,8 +370,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s"/>
       <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
@@ -451,7 +388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6">
       <c r="A2" t="n">
         <v>1</v>
       </c>
@@ -471,7 +408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6">
       <c r="A3" t="n">
         <v>2</v>
       </c>
@@ -491,7 +428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6">
       <c r="A4" t="n">
         <v>3</v>
       </c>
@@ -511,7 +448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6">
       <c r="A5" t="n">
         <v>4</v>
       </c>
@@ -531,7 +468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
@@ -552,6 +489,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test: update confMatrix in test data
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_confMatrix.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_confMatrix.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,10 +12,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54,22 +50,89 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -370,8 +433,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
@@ -388,7 +451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
@@ -396,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -408,27 +471,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
@@ -436,19 +499,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>39</v>
       </c>
       <c r="E4" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
@@ -456,19 +519,19 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E5" t="n">
         <v>63</v>
       </c>
       <c r="F5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
@@ -482,13 +545,13 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>